<commit_message>
removing 'Total' from labels
</commit_message>
<xml_diff>
--- a/median-income-hhsize/data/median-income-by-re-hhsize.xlsx
+++ b/median-income-hhsize/data/median-income-by-re-hhsize.xlsx
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Region</t>
   </si>
   <si>
-    <t xml:space="preserve">American Indian or Alaskan Native alone</t>
+    <t xml:space="preserve">American Indian or Alaskan Native</t>
   </si>
   <si>
     <t xml:space="preserve">detail</t>
@@ -76,43 +76,43 @@
     <t xml:space="preserve">single-person</t>
   </si>
   <si>
-    <t xml:space="preserve">Asian alone</t>
+    <t xml:space="preserve">Asian</t>
   </si>
   <si>
     <t xml:space="preserve">good</t>
   </si>
   <si>
-    <t xml:space="preserve">Black or African American alone</t>
+    <t xml:space="preserve">Black or African American</t>
   </si>
   <si>
     <t xml:space="preserve">Hispanic or Latino</t>
   </si>
   <si>
-    <t xml:space="preserve">Native Hawaiian and Other Pacific Islander alone</t>
+    <t xml:space="preserve">Native Hawaiian or Pacific Islander</t>
   </si>
   <si>
-    <t xml:space="preserve">Some Other Race alone</t>
+    <t xml:space="preserve">Some Other Race</t>
   </si>
   <si>
     <t xml:space="preserve">Two or More Races</t>
   </si>
   <si>
-    <t xml:space="preserve">White alone</t>
+    <t xml:space="preserve">White</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
   </si>
   <si>
-    <t xml:space="preserve">Total Multirace PSRC</t>
+    <t xml:space="preserve">Multirace PSRC</t>
   </si>
   <si>
-    <t xml:space="preserve">Total Single race PSRC</t>
+    <t xml:space="preserve">Single race PSRC</t>
   </si>
   <si>
-    <t xml:space="preserve">Total Single race Harvard</t>
+    <t xml:space="preserve">Single race Harvard</t>
   </si>
   <si>
-    <t xml:space="preserve">Total People of color</t>
+    <t xml:space="preserve">People of color</t>
   </si>
   <si>
     <t xml:space="preserve">King</t>
@@ -136,31 +136,31 @@
     <t xml:space="preserve">multi-person</t>
   </si>
   <si>
-    <t xml:space="preserve">Multiracial incl. Asian</t>
+    <t xml:space="preserve">MNAW</t>
   </si>
   <si>
-    <t xml:space="preserve">Multiracial incl. Asian, white</t>
+    <t xml:space="preserve">Multirace incl. Asian</t>
   </si>
   <si>
-    <t xml:space="preserve">Multiracial incl. white</t>
+    <t xml:space="preserve">Multirace incl. Asian, white</t>
   </si>
   <si>
-    <t xml:space="preserve">Multiracial not Asian or white</t>
+    <t xml:space="preserve">Multirace incl. white</t>
   </si>
   <si>
-    <t xml:space="preserve">Total Multirace Harvard</t>
+    <t xml:space="preserve">Multirace Harvard</t>
   </si>
   <si>
     <t xml:space="preserve">dichot</t>
   </si>
   <si>
-    <t xml:space="preserve">Multiracial not white</t>
+    <t xml:space="preserve">MNW</t>
   </si>
   <si>
     <t xml:space="preserve">single</t>
   </si>
   <si>
-    <t xml:space="preserve">Multiple Races</t>
+    <t xml:space="preserve">Multirace</t>
   </si>
 </sst>
 </file>
@@ -3865,17 +3865,17 @@
       </c>
       <c r="E11"/>
       <c r="F11" t="n">
-        <v>140840.9775</v>
+        <v>119396.055</v>
       </c>
       <c r="G11" t="n">
-        <v>135799.7976</v>
+        <v>110122.575</v>
       </c>
       <c r="H11"/>
       <c r="I11" t="n">
-        <v>5898.46796957727</v>
+        <v>4710.37812679202</v>
       </c>
       <c r="J11" t="n">
-        <v>8157.7013376749</v>
+        <v>8095.95197053973</v>
       </c>
       <c r="K11"/>
       <c r="L11" t="s">
@@ -3903,17 +3903,17 @@
       </c>
       <c r="E12"/>
       <c r="F12" t="n">
-        <v>181639.8848</v>
+        <v>140840.9775</v>
       </c>
       <c r="G12" t="n">
-        <v>182331.744</v>
+        <v>135799.7976</v>
       </c>
       <c r="H12"/>
       <c r="I12" t="n">
-        <v>5531.44262432623</v>
+        <v>5898.46796957727</v>
       </c>
       <c r="J12" t="n">
-        <v>5282.99897805594</v>
+        <v>8157.7013376749</v>
       </c>
       <c r="K12"/>
       <c r="L12" t="s">
@@ -3941,17 +3941,17 @@
       </c>
       <c r="E13"/>
       <c r="F13" t="n">
-        <v>142732.52</v>
+        <v>181639.8848</v>
       </c>
       <c r="G13" t="n">
-        <v>137233.384</v>
+        <v>182331.744</v>
       </c>
       <c r="H13"/>
       <c r="I13" t="n">
-        <v>3214.69867679675</v>
+        <v>5531.44262432623</v>
       </c>
       <c r="J13" t="n">
-        <v>3056.4370514043</v>
+        <v>5282.99897805594</v>
       </c>
       <c r="K13"/>
       <c r="L13" t="s">
@@ -3979,17 +3979,17 @@
       </c>
       <c r="E14"/>
       <c r="F14" t="n">
-        <v>119396.055</v>
+        <v>142732.52</v>
       </c>
       <c r="G14" t="n">
-        <v>110122.575</v>
+        <v>137233.384</v>
       </c>
       <c r="H14"/>
       <c r="I14" t="n">
-        <v>4710.37812679202</v>
+        <v>3214.69867679675</v>
       </c>
       <c r="J14" t="n">
-        <v>8095.95197053973</v>
+        <v>3056.4370514043</v>
       </c>
       <c r="K14"/>
       <c r="L14" t="s">
@@ -4627,17 +4627,17 @@
       </c>
       <c r="E29"/>
       <c r="F29" t="n">
-        <v>154456.977</v>
+        <v>126809.76</v>
       </c>
       <c r="G29" t="n">
-        <v>149869.146</v>
+        <v>113965.44</v>
       </c>
       <c r="H29"/>
       <c r="I29" t="n">
-        <v>11671.4010511167</v>
+        <v>13279.6880812759</v>
       </c>
       <c r="J29" t="n">
-        <v>14252.9722939988</v>
+        <v>15054.4025212806</v>
       </c>
       <c r="K29"/>
       <c r="L29" t="s">
@@ -4665,17 +4665,17 @@
       </c>
       <c r="E30"/>
       <c r="F30" t="n">
-        <v>210020.708</v>
+        <v>154456.977</v>
       </c>
       <c r="G30" t="n">
-        <v>210081.298</v>
+        <v>149869.146</v>
       </c>
       <c r="H30"/>
       <c r="I30" t="n">
-        <v>9268.32381610211</v>
+        <v>11671.4010511167</v>
       </c>
       <c r="J30" t="n">
-        <v>9406.80798793569</v>
+        <v>14252.9722939988</v>
       </c>
       <c r="K30"/>
       <c r="L30" t="s">
@@ -4703,17 +4703,17 @@
       </c>
       <c r="E31"/>
       <c r="F31" t="n">
-        <v>162796.2</v>
+        <v>210020.708</v>
       </c>
       <c r="G31" t="n">
-        <v>157005.772</v>
+        <v>210081.298</v>
       </c>
       <c r="H31"/>
       <c r="I31" t="n">
-        <v>5210.14226054</v>
+        <v>9268.32381610211</v>
       </c>
       <c r="J31" t="n">
-        <v>3611.42712030773</v>
+        <v>9406.80798793569</v>
       </c>
       <c r="K31"/>
       <c r="L31" t="s">
@@ -4741,17 +4741,17 @@
       </c>
       <c r="E32"/>
       <c r="F32" t="n">
-        <v>126809.76</v>
+        <v>162796.2</v>
       </c>
       <c r="G32" t="n">
-        <v>113965.44</v>
+        <v>157005.772</v>
       </c>
       <c r="H32"/>
       <c r="I32" t="n">
-        <v>13279.6880812759</v>
+        <v>5210.14226054</v>
       </c>
       <c r="J32" t="n">
-        <v>15054.4025212806</v>
+        <v>3611.42712030773</v>
       </c>
       <c r="K32"/>
       <c r="L32" t="s">
@@ -5389,24 +5389,24 @@
       </c>
       <c r="E47"/>
       <c r="F47" t="n">
-        <v>124756.6496</v>
+        <v>89717.584</v>
       </c>
       <c r="G47" t="n">
-        <v>100574.5008</v>
+        <v>83461.32</v>
       </c>
       <c r="H47"/>
       <c r="I47" t="n">
-        <v>60316.7915229755</v>
+        <v>21106.3659822485</v>
       </c>
       <c r="J47" t="n">
-        <v>36290.045118852</v>
+        <v>17655.4342195104</v>
       </c>
       <c r="K47"/>
       <c r="L47" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M47" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N47" t="s">
         <v>38</v>
@@ -5427,24 +5427,24 @@
       </c>
       <c r="E48"/>
       <c r="F48" t="n">
-        <v>128066.344</v>
+        <v>124756.6496</v>
       </c>
       <c r="G48" t="n">
-        <v>128066.344</v>
+        <v>100574.5008</v>
       </c>
       <c r="H48"/>
       <c r="I48" t="n">
-        <v>11286.4100202151</v>
+        <v>60316.7915229755</v>
       </c>
       <c r="J48" t="n">
-        <v>12150.6809649802</v>
+        <v>36290.045118852</v>
       </c>
       <c r="K48"/>
       <c r="L48" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M48" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N48" t="s">
         <v>38</v>
@@ -5465,17 +5465,17 @@
       </c>
       <c r="E49"/>
       <c r="F49" t="n">
-        <v>124605.48996</v>
+        <v>128066.344</v>
       </c>
       <c r="G49" t="n">
-        <v>122342.16</v>
+        <v>128066.344</v>
       </c>
       <c r="H49"/>
       <c r="I49" t="n">
-        <v>7273.04319156673</v>
+        <v>11286.4100202151</v>
       </c>
       <c r="J49" t="n">
-        <v>6818.74292609626</v>
+        <v>12150.6809649802</v>
       </c>
       <c r="K49"/>
       <c r="L49" t="s">
@@ -5503,17 +5503,17 @@
       </c>
       <c r="E50"/>
       <c r="F50" t="n">
-        <v>89717.584</v>
+        <v>124605.48996</v>
       </c>
       <c r="G50" t="n">
-        <v>83461.32</v>
+        <v>122342.16</v>
       </c>
       <c r="H50"/>
       <c r="I50" t="n">
-        <v>21106.3659822485</v>
+        <v>7273.04319156673</v>
       </c>
       <c r="J50" t="n">
-        <v>17655.4342195104</v>
+        <v>6818.74292609626</v>
       </c>
       <c r="K50"/>
       <c r="L50" t="s">
@@ -6151,17 +6151,17 @@
       </c>
       <c r="E65"/>
       <c r="F65" t="n">
-        <v>122342.16</v>
+        <v>115476.7712</v>
       </c>
       <c r="G65" t="n">
-        <v>112778.3</v>
+        <v>104326.65</v>
       </c>
       <c r="H65"/>
       <c r="I65" t="n">
-        <v>12615.9157730295</v>
+        <v>8443.58489337815</v>
       </c>
       <c r="J65" t="n">
-        <v>20874.7028658815</v>
+        <v>13519.2005684025</v>
       </c>
       <c r="K65"/>
       <c r="L65" t="s">
@@ -6189,17 +6189,17 @@
       </c>
       <c r="E66"/>
       <c r="F66" t="n">
-        <v>143586.2484</v>
+        <v>122342.16</v>
       </c>
       <c r="G66" t="n">
-        <v>142594.66</v>
+        <v>112778.3</v>
       </c>
       <c r="H66"/>
       <c r="I66" t="n">
-        <v>9059.30826934687</v>
+        <v>12615.9157730295</v>
       </c>
       <c r="J66" t="n">
-        <v>9217.00271115485</v>
+        <v>20874.7028658815</v>
       </c>
       <c r="K66"/>
       <c r="L66" t="s">
@@ -6227,17 +6227,17 @@
       </c>
       <c r="E67"/>
       <c r="F67" t="n">
-        <v>124381.196</v>
+        <v>143586.2484</v>
       </c>
       <c r="G67" t="n">
-        <v>119487.5096</v>
+        <v>142594.66</v>
       </c>
       <c r="H67"/>
       <c r="I67" t="n">
-        <v>5548.46485584311</v>
+        <v>9059.30826934687</v>
       </c>
       <c r="J67" t="n">
-        <v>5682.16595569948</v>
+        <v>9217.00271115485</v>
       </c>
       <c r="K67"/>
       <c r="L67" t="s">
@@ -6265,17 +6265,17 @@
       </c>
       <c r="E68"/>
       <c r="F68" t="n">
-        <v>115476.7712</v>
+        <v>124381.196</v>
       </c>
       <c r="G68" t="n">
-        <v>104326.65</v>
+        <v>119487.5096</v>
       </c>
       <c r="H68"/>
       <c r="I68" t="n">
-        <v>8443.58489337815</v>
+        <v>5548.46485584311</v>
       </c>
       <c r="J68" t="n">
-        <v>13519.2005684025</v>
+        <v>5682.16595569948</v>
       </c>
       <c r="K68"/>
       <c r="L68" t="s">
@@ -6913,17 +6913,17 @@
       </c>
       <c r="E83"/>
       <c r="F83" t="n">
-        <v>140082.52</v>
+        <v>120795.35424</v>
       </c>
       <c r="G83" t="n">
-        <v>138162.2528</v>
+        <v>120795.35424</v>
       </c>
       <c r="H83"/>
       <c r="I83" t="n">
-        <v>14754.7142184667</v>
+        <v>10941.8075530846</v>
       </c>
       <c r="J83" t="n">
-        <v>14613.8334319742</v>
+        <v>11811.7006629493</v>
       </c>
       <c r="K83"/>
       <c r="L83" t="s">
@@ -6951,17 +6951,17 @@
       </c>
       <c r="E84"/>
       <c r="F84" t="n">
-        <v>158535.049</v>
+        <v>140082.52</v>
       </c>
       <c r="G84" t="n">
-        <v>161695.5548</v>
+        <v>138162.2528</v>
       </c>
       <c r="H84"/>
       <c r="I84" t="n">
-        <v>11170.355008284</v>
+        <v>14754.7142184667</v>
       </c>
       <c r="J84" t="n">
-        <v>13235.2415473843</v>
+        <v>14613.8334319742</v>
       </c>
       <c r="K84"/>
       <c r="L84" t="s">
@@ -6989,17 +6989,17 @@
       </c>
       <c r="E85"/>
       <c r="F85" t="n">
-        <v>139102.2</v>
+        <v>158535.049</v>
       </c>
       <c r="G85" t="n">
-        <v>134465.46</v>
+        <v>161695.5548</v>
       </c>
       <c r="H85"/>
       <c r="I85" t="n">
-        <v>4776.38938367235</v>
+        <v>11170.355008284</v>
       </c>
       <c r="J85" t="n">
-        <v>4876.52608549957</v>
+        <v>13235.2415473843</v>
       </c>
       <c r="K85"/>
       <c r="L85" t="s">
@@ -7027,17 +7027,17 @@
       </c>
       <c r="E86"/>
       <c r="F86" t="n">
-        <v>120795.35424</v>
+        <v>139102.2</v>
       </c>
       <c r="G86" t="n">
-        <v>120795.35424</v>
+        <v>134465.46</v>
       </c>
       <c r="H86"/>
       <c r="I86" t="n">
-        <v>10941.8075530846</v>
+        <v>4776.38938367235</v>
       </c>
       <c r="J86" t="n">
-        <v>11811.7006629493</v>
+        <v>4876.52608549957</v>
       </c>
       <c r="K86"/>
       <c r="L86" t="s">
@@ -10644,24 +10644,24 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
         <v>44</v>
       </c>
       <c r="E11"/>
       <c r="F11" t="n">
-        <v>151943.12</v>
+        <v>127439.75</v>
       </c>
       <c r="G11" t="n">
-        <v>146978.5504</v>
+        <v>121322.642</v>
       </c>
       <c r="H11"/>
       <c r="I11" t="n">
-        <v>2424.27453418516</v>
+        <v>3616.45776563897</v>
       </c>
       <c r="J11" t="n">
-        <v>2466.30163200838</v>
+        <v>4184.43722363556</v>
       </c>
       <c r="K11"/>
       <c r="L11" t="s">
@@ -10682,24 +10682,24 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
         <v>44</v>
       </c>
       <c r="E12"/>
       <c r="F12" t="n">
-        <v>127439.75</v>
+        <v>151943.12</v>
       </c>
       <c r="G12" t="n">
-        <v>121322.642</v>
+        <v>146978.5504</v>
       </c>
       <c r="H12"/>
       <c r="I12" t="n">
-        <v>3616.45776563897</v>
+        <v>2424.27453418516</v>
       </c>
       <c r="J12" t="n">
-        <v>4184.43722363556</v>
+        <v>2466.30163200838</v>
       </c>
       <c r="K12"/>
       <c r="L12" t="s">
@@ -11330,24 +11330,24 @@
         <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D27" t="s">
         <v>44</v>
       </c>
       <c r="E27"/>
       <c r="F27" t="n">
-        <v>176376.614</v>
+        <v>135799.7976</v>
       </c>
       <c r="G27" t="n">
-        <v>173318.06</v>
+        <v>129274.8824</v>
       </c>
       <c r="H27"/>
       <c r="I27" t="n">
-        <v>3905.00667229531</v>
+        <v>7893.34572076315</v>
       </c>
       <c r="J27" t="n">
-        <v>3719.69697294347</v>
+        <v>4741.50341510183</v>
       </c>
       <c r="K27"/>
       <c r="L27" t="s">
@@ -11368,24 +11368,24 @@
         <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
         <v>44</v>
       </c>
       <c r="E28"/>
       <c r="F28" t="n">
-        <v>135799.7976</v>
+        <v>176376.614</v>
       </c>
       <c r="G28" t="n">
-        <v>129274.8824</v>
+        <v>173318.06</v>
       </c>
       <c r="H28"/>
       <c r="I28" t="n">
-        <v>7893.34572076315</v>
+        <v>3905.00667229531</v>
       </c>
       <c r="J28" t="n">
-        <v>4741.50341510183</v>
+        <v>3719.69697294347</v>
       </c>
       <c r="K28"/>
       <c r="L28" t="s">
@@ -12016,24 +12016,24 @@
         <v>34</v>
       </c>
       <c r="C43" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D43" t="s">
         <v>44</v>
       </c>
       <c r="E43"/>
       <c r="F43" t="n">
-        <v>125539.7355</v>
+        <v>94971.2</v>
       </c>
       <c r="G43" t="n">
-        <v>124605.48996</v>
+        <v>92269.1968</v>
       </c>
       <c r="H43"/>
       <c r="I43" t="n">
-        <v>5964.11235258241</v>
+        <v>20572.5644878137</v>
       </c>
       <c r="J43" t="n">
-        <v>5287.60700133882</v>
+        <v>11252.6838684979</v>
       </c>
       <c r="K43"/>
       <c r="L43" t="s">
@@ -12054,24 +12054,24 @@
         <v>34</v>
       </c>
       <c r="C44" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D44" t="s">
         <v>44</v>
       </c>
       <c r="E44"/>
       <c r="F44" t="n">
-        <v>94971.2</v>
+        <v>125539.7355</v>
       </c>
       <c r="G44" t="n">
-        <v>92269.1968</v>
+        <v>124605.48996</v>
       </c>
       <c r="H44"/>
       <c r="I44" t="n">
-        <v>20572.5644878137</v>
+        <v>5964.11235258241</v>
       </c>
       <c r="J44" t="n">
-        <v>11252.6838684979</v>
+        <v>5287.60700133882</v>
       </c>
       <c r="K44"/>
       <c r="L44" t="s">
@@ -12702,24 +12702,24 @@
         <v>36</v>
       </c>
       <c r="C59" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D59" t="s">
         <v>44</v>
       </c>
       <c r="E59"/>
       <c r="F59" t="n">
-        <v>127510.35</v>
+        <v>117807.97155</v>
       </c>
       <c r="G59" t="n">
-        <v>124810.42</v>
+        <v>107890.46828</v>
       </c>
       <c r="H59"/>
       <c r="I59" t="n">
-        <v>3842.17296623472</v>
+        <v>7203.52450750144</v>
       </c>
       <c r="J59" t="n">
-        <v>4550.57762723557</v>
+        <v>11763.2228693812</v>
       </c>
       <c r="K59"/>
       <c r="L59" t="s">
@@ -12740,24 +12740,24 @@
         <v>36</v>
       </c>
       <c r="C60" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D60" t="s">
         <v>44</v>
       </c>
       <c r="E60"/>
       <c r="F60" t="n">
-        <v>117807.97155</v>
+        <v>127510.35</v>
       </c>
       <c r="G60" t="n">
-        <v>107890.46828</v>
+        <v>124810.42</v>
       </c>
       <c r="H60"/>
       <c r="I60" t="n">
-        <v>7203.52450750144</v>
+        <v>3842.17296623472</v>
       </c>
       <c r="J60" t="n">
-        <v>11763.2228693812</v>
+        <v>4550.57762723557</v>
       </c>
       <c r="K60"/>
       <c r="L60" t="s">
@@ -13388,24 +13388,24 @@
         <v>37</v>
       </c>
       <c r="C75" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D75" t="s">
         <v>44</v>
       </c>
       <c r="E75"/>
       <c r="F75" t="n">
-        <v>142456.8</v>
+        <v>125771.5725</v>
       </c>
       <c r="G75" t="n">
-        <v>139797.711</v>
+        <v>124810.42</v>
       </c>
       <c r="H75"/>
       <c r="I75" t="n">
-        <v>2399.1500464149</v>
+        <v>5845.09900412048</v>
       </c>
       <c r="J75" t="n">
-        <v>2558.74058501535</v>
+        <v>5567.97138771177</v>
       </c>
       <c r="K75"/>
       <c r="L75" t="s">
@@ -13426,24 +13426,24 @@
         <v>37</v>
       </c>
       <c r="C76" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D76" t="s">
         <v>44</v>
       </c>
       <c r="E76"/>
       <c r="F76" t="n">
-        <v>125771.5725</v>
+        <v>142456.8</v>
       </c>
       <c r="G76" t="n">
-        <v>124810.42</v>
+        <v>139797.711</v>
       </c>
       <c r="H76"/>
       <c r="I76" t="n">
-        <v>5845.09900412048</v>
+        <v>2399.1500464149</v>
       </c>
       <c r="J76" t="n">
-        <v>5567.97138771177</v>
+        <v>2558.74058501535</v>
       </c>
       <c r="K76"/>
       <c r="L76" t="s">

</xml_diff>

<commit_message>
adding NA rows for missing geography/race combos
</commit_message>
<xml_diff>
--- a/median-income-hhsize/data/median-income-by-re-hhsize.xlsx
+++ b/median-income-hhsize/data/median-income-by-re-hhsize.xlsx
@@ -94,13 +94,13 @@
     <t xml:space="preserve">Some Other Race</t>
   </si>
   <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
     <t xml:space="preserve">Two or More Races</t>
   </si>
   <si>
     <t xml:space="preserve">White</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
   </si>
   <si>
     <t xml:space="preserve">Multirace PSRC</t>
@@ -814,22 +814,22 @@
         <v>16</v>
       </c>
       <c r="E8" t="n">
-        <v>54191.89875</v>
+        <v>57959.25</v>
       </c>
       <c r="F8" t="n">
-        <v>54191.89875</v>
+        <v>57959.25</v>
       </c>
       <c r="G8" t="n">
-        <v>54191.89875</v>
+        <v>57959.25</v>
       </c>
       <c r="H8" t="n">
-        <v>3125.25308491457</v>
+        <v>1264.48170014687</v>
       </c>
       <c r="I8" t="n">
-        <v>3125.25308491457</v>
+        <v>1028.22535144888</v>
       </c>
       <c r="J8" t="n">
-        <v>3125.25308491457</v>
+        <v>1264.48170014687</v>
       </c>
       <c r="K8" t="s">
         <v>20</v>
@@ -858,22 +858,22 @@
         <v>16</v>
       </c>
       <c r="E9" t="n">
-        <v>57487.0912</v>
+        <v>54191.89875</v>
       </c>
       <c r="F9" t="n">
-        <v>57521.324</v>
+        <v>54191.89875</v>
       </c>
       <c r="G9" t="n">
-        <v>57487.0912</v>
+        <v>54191.89875</v>
       </c>
       <c r="H9" t="n">
-        <v>1253.34432695792</v>
+        <v>3125.25308491457</v>
       </c>
       <c r="I9" t="n">
-        <v>1209.8527365922</v>
+        <v>3125.25308491457</v>
       </c>
       <c r="J9" t="n">
-        <v>1253.34432695792</v>
+        <v>3125.25308491457</v>
       </c>
       <c r="K9" t="s">
         <v>20</v>
@@ -902,22 +902,22 @@
         <v>16</v>
       </c>
       <c r="E10" t="n">
-        <v>57959.25</v>
+        <v>57487.0912</v>
       </c>
       <c r="F10" t="n">
-        <v>57959.25</v>
+        <v>57521.324</v>
       </c>
       <c r="G10" t="n">
-        <v>57959.25</v>
+        <v>57487.0912</v>
       </c>
       <c r="H10" t="n">
-        <v>1264.48170014687</v>
+        <v>1253.34432695792</v>
       </c>
       <c r="I10" t="n">
-        <v>1028.22535144888</v>
+        <v>1209.8527365922</v>
       </c>
       <c r="J10" t="n">
-        <v>1264.48170014687</v>
+        <v>1253.34432695792</v>
       </c>
       <c r="K10" t="s">
         <v>20</v>
@@ -1386,22 +1386,22 @@
         <v>16</v>
       </c>
       <c r="E21" t="n">
-        <v>55350.708</v>
+        <v>64105.56</v>
       </c>
       <c r="F21" t="n">
-        <v>55350.708</v>
+        <v>64331.5858</v>
       </c>
       <c r="G21" t="n">
-        <v>55350.708</v>
+        <v>64105.56</v>
       </c>
       <c r="H21" t="n">
-        <v>5917.02153301515</v>
+        <v>2214.60709266114</v>
       </c>
       <c r="I21" t="n">
-        <v>5917.02153301515</v>
+        <v>2114.88132442924</v>
       </c>
       <c r="J21" t="n">
-        <v>5917.02153301515</v>
+        <v>2214.60709266114</v>
       </c>
       <c r="K21" t="s">
         <v>20</v>
@@ -1430,22 +1430,22 @@
         <v>16</v>
       </c>
       <c r="E22" t="n">
-        <v>64817.844</v>
+        <v>55350.708</v>
       </c>
       <c r="F22" t="n">
-        <v>64854.1344</v>
+        <v>55350.708</v>
       </c>
       <c r="G22" t="n">
-        <v>64817.844</v>
+        <v>55350.708</v>
       </c>
       <c r="H22" t="n">
-        <v>2162.62587050882</v>
+        <v>5917.02153301515</v>
       </c>
       <c r="I22" t="n">
-        <v>2025.48263815248</v>
+        <v>5917.02153301515</v>
       </c>
       <c r="J22" t="n">
-        <v>2162.62587050882</v>
+        <v>5917.02153301515</v>
       </c>
       <c r="K22" t="s">
         <v>20</v>
@@ -1474,22 +1474,22 @@
         <v>16</v>
       </c>
       <c r="E23" t="n">
-        <v>64105.56</v>
+        <v>64817.844</v>
       </c>
       <c r="F23" t="n">
-        <v>64331.5858</v>
+        <v>64854.1344</v>
       </c>
       <c r="G23" t="n">
-        <v>64105.56</v>
+        <v>64817.844</v>
       </c>
       <c r="H23" t="n">
-        <v>2214.60709266114</v>
+        <v>2162.62587050882</v>
       </c>
       <c r="I23" t="n">
-        <v>2114.88132442924</v>
+        <v>2025.48263815248</v>
       </c>
       <c r="J23" t="n">
-        <v>2214.60709266114</v>
+        <v>2162.62587050882</v>
       </c>
       <c r="K23" t="s">
         <v>20</v>
@@ -1958,31 +1958,31 @@
         <v>16</v>
       </c>
       <c r="E34" t="n">
-        <v>62730.8024</v>
+        <v>49147.596</v>
       </c>
       <c r="F34" t="n">
-        <v>62730.8024</v>
+        <v>49171.35314</v>
       </c>
       <c r="G34" t="n">
-        <v>62730.8024</v>
+        <v>49147.596</v>
       </c>
       <c r="H34" t="n">
-        <v>20746.1460009376</v>
+        <v>2717.26132515061</v>
       </c>
       <c r="I34" t="n">
-        <v>20746.1460009376</v>
+        <v>2734.44430974366</v>
       </c>
       <c r="J34" t="n">
-        <v>20746.1460009376</v>
+        <v>2717.26132515061</v>
       </c>
       <c r="K34" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L34" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M34" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N34" t="s">
         <v>18</v>
@@ -2002,31 +2002,31 @@
         <v>16</v>
       </c>
       <c r="E35" t="n">
-        <v>49171.35314</v>
+        <v>62730.8024</v>
       </c>
       <c r="F35" t="n">
-        <v>49171.35314</v>
+        <v>62730.8024</v>
       </c>
       <c r="G35" t="n">
-        <v>49171.35314</v>
+        <v>62730.8024</v>
       </c>
       <c r="H35" t="n">
-        <v>2917.94605346304</v>
+        <v>20746.1460009376</v>
       </c>
       <c r="I35" t="n">
-        <v>2962.98381458141</v>
+        <v>20746.1460009376</v>
       </c>
       <c r="J35" t="n">
-        <v>2917.94605346304</v>
+        <v>20746.1460009376</v>
       </c>
       <c r="K35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N35" t="s">
         <v>18</v>
@@ -2046,22 +2046,22 @@
         <v>16</v>
       </c>
       <c r="E36" t="n">
-        <v>49147.596</v>
+        <v>49171.35314</v>
       </c>
       <c r="F36" t="n">
         <v>49171.35314</v>
       </c>
       <c r="G36" t="n">
-        <v>49147.596</v>
+        <v>49171.35314</v>
       </c>
       <c r="H36" t="n">
-        <v>2717.26132515061</v>
+        <v>2917.94605346304</v>
       </c>
       <c r="I36" t="n">
-        <v>2734.44430974366</v>
+        <v>2962.98381458141</v>
       </c>
       <c r="J36" t="n">
-        <v>2717.26132515061</v>
+        <v>2917.94605346304</v>
       </c>
       <c r="K36" t="s">
         <v>20</v>
@@ -2530,22 +2530,22 @@
         <v>16</v>
       </c>
       <c r="E47" t="n">
-        <v>53322.51</v>
+        <v>49844.955</v>
       </c>
       <c r="F47" t="n">
-        <v>53322.51</v>
+        <v>49844.955</v>
       </c>
       <c r="G47" t="n">
-        <v>53322.51</v>
+        <v>49844.955</v>
       </c>
       <c r="H47" t="n">
-        <v>9859.83185896309</v>
+        <v>1900.05386102308</v>
       </c>
       <c r="I47" t="n">
-        <v>9859.83185896309</v>
+        <v>1880.39830998911</v>
       </c>
       <c r="J47" t="n">
-        <v>9859.83185896309</v>
+        <v>1900.05386102308</v>
       </c>
       <c r="K47" t="s">
         <v>20</v>
@@ -2574,22 +2574,22 @@
         <v>16</v>
       </c>
       <c r="E48" t="n">
-        <v>50683.8836</v>
+        <v>53322.51</v>
       </c>
       <c r="F48" t="n">
-        <v>50723.904</v>
+        <v>53322.51</v>
       </c>
       <c r="G48" t="n">
-        <v>50683.8836</v>
+        <v>53322.51</v>
       </c>
       <c r="H48" t="n">
-        <v>2822.14856241887</v>
+        <v>9859.83185896309</v>
       </c>
       <c r="I48" t="n">
-        <v>2842.41542380844</v>
+        <v>9859.83185896309</v>
       </c>
       <c r="J48" t="n">
-        <v>2822.14856241887</v>
+        <v>9859.83185896309</v>
       </c>
       <c r="K48" t="s">
         <v>20</v>
@@ -2618,22 +2618,22 @@
         <v>16</v>
       </c>
       <c r="E49" t="n">
-        <v>49844.955</v>
+        <v>50683.8836</v>
       </c>
       <c r="F49" t="n">
-        <v>49844.955</v>
+        <v>50723.904</v>
       </c>
       <c r="G49" t="n">
-        <v>49844.955</v>
+        <v>50683.8836</v>
       </c>
       <c r="H49" t="n">
-        <v>1900.05386102308</v>
+        <v>2822.14856241887</v>
       </c>
       <c r="I49" t="n">
-        <v>1880.39830998911</v>
+        <v>2842.41542380844</v>
       </c>
       <c r="J49" t="n">
-        <v>1900.05386102308</v>
+        <v>2822.14856241887</v>
       </c>
       <c r="K49" t="s">
         <v>20</v>
@@ -3102,22 +3102,22 @@
         <v>16</v>
       </c>
       <c r="E60" t="n">
-        <v>48936.864</v>
+        <v>50975.9</v>
       </c>
       <c r="F60" t="n">
-        <v>48936.864</v>
+        <v>51004.14</v>
       </c>
       <c r="G60" t="n">
-        <v>48936.864</v>
+        <v>50975.9</v>
       </c>
       <c r="H60" t="n">
-        <v>8412.2346187217</v>
+        <v>2566.40103174919</v>
       </c>
       <c r="I60" t="n">
-        <v>8412.2346187217</v>
+        <v>2623.1295232966</v>
       </c>
       <c r="J60" t="n">
-        <v>8412.2346187217</v>
+        <v>2566.40103174919</v>
       </c>
       <c r="K60" t="s">
         <v>20</v>
@@ -3146,22 +3146,22 @@
         <v>16</v>
       </c>
       <c r="E61" t="n">
-        <v>50975.9</v>
+        <v>48936.864</v>
       </c>
       <c r="F61" t="n">
-        <v>50975.9</v>
+        <v>48936.864</v>
       </c>
       <c r="G61" t="n">
-        <v>50975.9</v>
+        <v>48936.864</v>
       </c>
       <c r="H61" t="n">
-        <v>3326.3870604713</v>
+        <v>8412.2346187217</v>
       </c>
       <c r="I61" t="n">
-        <v>3295.86949196496</v>
+        <v>8412.2346187217</v>
       </c>
       <c r="J61" t="n">
-        <v>3326.3870604713</v>
+        <v>8412.2346187217</v>
       </c>
       <c r="K61" t="s">
         <v>20</v>
@@ -3193,19 +3193,19 @@
         <v>50975.9</v>
       </c>
       <c r="F62" t="n">
-        <v>51004.14</v>
+        <v>50975.9</v>
       </c>
       <c r="G62" t="n">
         <v>50975.9</v>
       </c>
       <c r="H62" t="n">
-        <v>2566.40103174919</v>
+        <v>3326.3870604713</v>
       </c>
       <c r="I62" t="n">
-        <v>2623.1295232966</v>
+        <v>3295.86949196496</v>
       </c>
       <c r="J62" t="n">
-        <v>2566.40103174919</v>
+        <v>3326.3870604713</v>
       </c>
       <c r="K62" t="s">
         <v>20</v>
@@ -3732,22 +3732,22 @@
         <v>16</v>
       </c>
       <c r="E8" t="n">
-        <v>126809.76</v>
+        <v>136521.1</v>
       </c>
       <c r="F8" t="n">
-        <v>100849.095</v>
+        <v>136521.1</v>
       </c>
       <c r="G8" t="n">
-        <v>107486.368</v>
+        <v>136521.1</v>
       </c>
       <c r="H8" t="n">
-        <v>4332.25277201833</v>
+        <v>1066.12046660227</v>
       </c>
       <c r="I8" t="n">
-        <v>6428.32084072217</v>
+        <v>1085.28363716262</v>
       </c>
       <c r="J8" t="n">
-        <v>8227.9137695208</v>
+        <v>1066.12046660227</v>
       </c>
       <c r="K8" t="s">
         <v>20</v>
@@ -3776,22 +3776,22 @@
         <v>16</v>
       </c>
       <c r="E9" t="n">
-        <v>142732.52</v>
+        <v>126809.76</v>
       </c>
       <c r="F9" t="n">
-        <v>140840.9775</v>
+        <v>100849.095</v>
       </c>
       <c r="G9" t="n">
-        <v>141652.407</v>
+        <v>107486.368</v>
       </c>
       <c r="H9" t="n">
-        <v>1428.63578540444</v>
+        <v>4332.25277201833</v>
       </c>
       <c r="I9" t="n">
-        <v>1479.34869364543</v>
+        <v>6428.32084072217</v>
       </c>
       <c r="J9" t="n">
-        <v>1460.92572429665</v>
+        <v>8227.9137695208</v>
       </c>
       <c r="K9" t="s">
         <v>20</v>
@@ -3820,22 +3820,22 @@
         <v>16</v>
       </c>
       <c r="E10" t="n">
-        <v>136521.1</v>
+        <v>142732.52</v>
       </c>
       <c r="F10" t="n">
-        <v>136521.1</v>
+        <v>140840.9775</v>
       </c>
       <c r="G10" t="n">
-        <v>136521.1</v>
+        <v>141652.407</v>
       </c>
       <c r="H10" t="n">
-        <v>1066.12046660227</v>
+        <v>1428.63578540444</v>
       </c>
       <c r="I10" t="n">
-        <v>1085.28363716262</v>
+        <v>1479.34869364543</v>
       </c>
       <c r="J10" t="n">
-        <v>1066.12046660227</v>
+        <v>1460.92572429665</v>
       </c>
       <c r="K10" t="s">
         <v>20</v>
@@ -4494,22 +4494,22 @@
         <v>16</v>
       </c>
       <c r="E26" t="n">
-        <v>142834.4718</v>
+        <v>156489.975</v>
       </c>
       <c r="F26" t="n">
-        <v>109088.426</v>
+        <v>156489.975</v>
       </c>
       <c r="G26" t="n">
-        <v>122393.1359</v>
+        <v>156489.975</v>
       </c>
       <c r="H26" t="n">
-        <v>10577.2385772801</v>
+        <v>1800.43590264081</v>
       </c>
       <c r="I26" t="n">
-        <v>12096.2742091487</v>
+        <v>1788.75431262822</v>
       </c>
       <c r="J26" t="n">
-        <v>20177.7621517745</v>
+        <v>1800.43590264081</v>
       </c>
       <c r="K26" t="s">
         <v>20</v>
@@ -4538,22 +4538,22 @@
         <v>16</v>
       </c>
       <c r="E27" t="n">
-        <v>168220.47</v>
+        <v>142834.4718</v>
       </c>
       <c r="F27" t="n">
-        <v>165012.46</v>
+        <v>109088.426</v>
       </c>
       <c r="G27" t="n">
-        <v>165943.5932</v>
+        <v>122393.1359</v>
       </c>
       <c r="H27" t="n">
-        <v>2504.44178656926</v>
+        <v>10577.2385772801</v>
       </c>
       <c r="I27" t="n">
-        <v>2845.95886728038</v>
+        <v>12096.2742091487</v>
       </c>
       <c r="J27" t="n">
-        <v>2986.07009140882</v>
+        <v>20177.7621517745</v>
       </c>
       <c r="K27" t="s">
         <v>20</v>
@@ -4582,22 +4582,22 @@
         <v>16</v>
       </c>
       <c r="E28" t="n">
-        <v>156489.975</v>
+        <v>168220.47</v>
       </c>
       <c r="F28" t="n">
-        <v>156489.975</v>
+        <v>165012.46</v>
       </c>
       <c r="G28" t="n">
-        <v>156489.975</v>
+        <v>165943.5932</v>
       </c>
       <c r="H28" t="n">
-        <v>1800.43590264081</v>
+        <v>2504.44178656926</v>
       </c>
       <c r="I28" t="n">
-        <v>1788.75431262822</v>
+        <v>2845.95886728038</v>
       </c>
       <c r="J28" t="n">
-        <v>1800.43590264081</v>
+        <v>2986.07009140882</v>
       </c>
       <c r="K28" t="s">
         <v>20</v>
@@ -5256,22 +5256,22 @@
         <v>16</v>
       </c>
       <c r="E44" t="n">
-        <v>94815.174</v>
+        <v>118298.572</v>
       </c>
       <c r="F44" t="n">
-        <v>94937.2515</v>
+        <v>118298.572</v>
       </c>
       <c r="G44" t="n">
-        <v>95507.104</v>
+        <v>118298.572</v>
       </c>
       <c r="H44" t="n">
-        <v>6342.65022080927</v>
+        <v>3383.90722201948</v>
       </c>
       <c r="I44" t="n">
-        <v>14638.3239283411</v>
+        <v>3383.90722201948</v>
       </c>
       <c r="J44" t="n">
-        <v>12435.8630344971</v>
+        <v>3383.90722201948</v>
       </c>
       <c r="K44" t="s">
         <v>20</v>
@@ -5300,22 +5300,22 @@
         <v>16</v>
       </c>
       <c r="E45" t="n">
-        <v>121598.5065</v>
+        <v>94815.174</v>
       </c>
       <c r="F45" t="n">
-        <v>120771.2</v>
+        <v>94937.2515</v>
       </c>
       <c r="G45" t="n">
-        <v>121088.28</v>
+        <v>95507.104</v>
       </c>
       <c r="H45" t="n">
-        <v>3029.87727404456</v>
+        <v>6342.65022080927</v>
       </c>
       <c r="I45" t="n">
-        <v>3502.54364546422</v>
+        <v>14638.3239283411</v>
       </c>
       <c r="J45" t="n">
-        <v>3564.59376476758</v>
+        <v>12435.8630344971</v>
       </c>
       <c r="K45" t="s">
         <v>20</v>
@@ -5344,22 +5344,22 @@
         <v>16</v>
       </c>
       <c r="E46" t="n">
-        <v>118298.572</v>
+        <v>121598.5065</v>
       </c>
       <c r="F46" t="n">
-        <v>118298.572</v>
+        <v>120771.2</v>
       </c>
       <c r="G46" t="n">
-        <v>118298.572</v>
+        <v>121088.28</v>
       </c>
       <c r="H46" t="n">
-        <v>3383.90722201948</v>
+        <v>3029.87727404456</v>
       </c>
       <c r="I46" t="n">
-        <v>3383.90722201948</v>
+        <v>3502.54364546422</v>
       </c>
       <c r="J46" t="n">
-        <v>3383.90722201948</v>
+        <v>3564.59376476758</v>
       </c>
       <c r="K46" t="s">
         <v>20</v>
@@ -6018,22 +6018,22 @@
         <v>16</v>
       </c>
       <c r="E62" t="n">
-        <v>103990.836</v>
+        <v>115222.989</v>
       </c>
       <c r="F62" t="n">
-        <v>80916.704</v>
+        <v>115222.989</v>
       </c>
       <c r="G62" t="n">
-        <v>82150.088</v>
+        <v>115222.989</v>
       </c>
       <c r="H62" t="n">
-        <v>8843.18489533869</v>
+        <v>1829.92844779909</v>
       </c>
       <c r="I62" t="n">
-        <v>7753.56910572762</v>
+        <v>1841.65328029918</v>
       </c>
       <c r="J62" t="n">
-        <v>9514.16986203294</v>
+        <v>1829.92844779909</v>
       </c>
       <c r="K62" t="s">
         <v>20</v>
@@ -6062,22 +6062,22 @@
         <v>16</v>
       </c>
       <c r="E63" t="n">
-        <v>121978.912</v>
+        <v>103990.836</v>
       </c>
       <c r="F63" t="n">
-        <v>120555.24</v>
+        <v>80916.704</v>
       </c>
       <c r="G63" t="n">
-        <v>121088.28</v>
+        <v>82150.088</v>
       </c>
       <c r="H63" t="n">
-        <v>2248.58898249227</v>
+        <v>8843.18489533869</v>
       </c>
       <c r="I63" t="n">
-        <v>2103.89340159665</v>
+        <v>7753.56910572762</v>
       </c>
       <c r="J63" t="n">
-        <v>2164.21133347385</v>
+        <v>9514.16986203294</v>
       </c>
       <c r="K63" t="s">
         <v>20</v>
@@ -6106,22 +6106,22 @@
         <v>16</v>
       </c>
       <c r="E64" t="n">
-        <v>115222.989</v>
+        <v>121978.912</v>
       </c>
       <c r="F64" t="n">
-        <v>115222.989</v>
+        <v>120555.24</v>
       </c>
       <c r="G64" t="n">
-        <v>115222.989</v>
+        <v>121088.28</v>
       </c>
       <c r="H64" t="n">
-        <v>1829.92844779909</v>
+        <v>2248.58898249227</v>
       </c>
       <c r="I64" t="n">
-        <v>1841.65328029918</v>
+        <v>2103.89340159665</v>
       </c>
       <c r="J64" t="n">
-        <v>1829.92844779909</v>
+        <v>2164.21133347385</v>
       </c>
       <c r="K64" t="s">
         <v>20</v>
@@ -6780,22 +6780,22 @@
         <v>16</v>
       </c>
       <c r="E80" t="n">
-        <v>129315.219</v>
+        <v>129478.786</v>
       </c>
       <c r="F80" t="n">
-        <v>118951.428</v>
+        <v>129478.786</v>
       </c>
       <c r="G80" t="n">
-        <v>119544.998</v>
+        <v>129478.786</v>
       </c>
       <c r="H80" t="n">
-        <v>7933.14150963542</v>
+        <v>2650.9311255005</v>
       </c>
       <c r="I80" t="n">
-        <v>10525.5474188639</v>
+        <v>2650.9311255005</v>
       </c>
       <c r="J80" t="n">
-        <v>12155.1133818182</v>
+        <v>2650.9311255005</v>
       </c>
       <c r="K80" t="s">
         <v>20</v>
@@ -6824,22 +6824,22 @@
         <v>16</v>
       </c>
       <c r="E81" t="n">
-        <v>131517.822</v>
+        <v>129315.219</v>
       </c>
       <c r="F81" t="n">
-        <v>129828.72</v>
+        <v>118951.428</v>
       </c>
       <c r="G81" t="n">
-        <v>130229.258</v>
+        <v>119544.998</v>
       </c>
       <c r="H81" t="n">
-        <v>2659.93321186545</v>
+        <v>7933.14150963542</v>
       </c>
       <c r="I81" t="n">
-        <v>3072.44619562329</v>
+        <v>10525.5474188639</v>
       </c>
       <c r="J81" t="n">
-        <v>2930.76839293921</v>
+        <v>12155.1133818182</v>
       </c>
       <c r="K81" t="s">
         <v>20</v>
@@ -6868,22 +6868,22 @@
         <v>16</v>
       </c>
       <c r="E82" t="n">
-        <v>129478.786</v>
+        <v>131517.822</v>
       </c>
       <c r="F82" t="n">
-        <v>129478.786</v>
+        <v>129828.72</v>
       </c>
       <c r="G82" t="n">
-        <v>129478.786</v>
+        <v>130229.258</v>
       </c>
       <c r="H82" t="n">
-        <v>2650.9311255005</v>
+        <v>2659.93321186545</v>
       </c>
       <c r="I82" t="n">
-        <v>2650.9311255005</v>
+        <v>3072.44619562329</v>
       </c>
       <c r="J82" t="n">
-        <v>2650.9311255005</v>
+        <v>2930.76839293921</v>
       </c>
       <c r="K82" t="s">
         <v>20</v>
@@ -7600,22 +7600,22 @@
         <v>44</v>
       </c>
       <c r="E8" t="n">
-        <v>54191.89875</v>
+        <v>57959.25</v>
       </c>
       <c r="F8" t="n">
-        <v>54191.89875</v>
+        <v>57959.25</v>
       </c>
       <c r="G8" t="n">
-        <v>54191.89875</v>
+        <v>57959.25</v>
       </c>
       <c r="H8" t="n">
-        <v>3125.25308491457</v>
+        <v>1264.48170014687</v>
       </c>
       <c r="I8" t="n">
-        <v>3125.25308491457</v>
+        <v>1028.22535144888</v>
       </c>
       <c r="J8" t="n">
-        <v>3125.25308491457</v>
+        <v>1264.48170014687</v>
       </c>
       <c r="K8" t="s">
         <v>20</v>
@@ -7644,22 +7644,22 @@
         <v>44</v>
       </c>
       <c r="E9" t="n">
-        <v>57487.0912</v>
+        <v>54191.89875</v>
       </c>
       <c r="F9" t="n">
-        <v>57521.324</v>
+        <v>54191.89875</v>
       </c>
       <c r="G9" t="n">
-        <v>57487.0912</v>
+        <v>54191.89875</v>
       </c>
       <c r="H9" t="n">
-        <v>1253.34432695792</v>
+        <v>3125.25308491457</v>
       </c>
       <c r="I9" t="n">
-        <v>1209.8527365922</v>
+        <v>3125.25308491457</v>
       </c>
       <c r="J9" t="n">
-        <v>1253.34432695792</v>
+        <v>3125.25308491457</v>
       </c>
       <c r="K9" t="s">
         <v>20</v>
@@ -7688,22 +7688,22 @@
         <v>44</v>
       </c>
       <c r="E10" t="n">
-        <v>57959.25</v>
+        <v>57487.0912</v>
       </c>
       <c r="F10" t="n">
-        <v>57959.25</v>
+        <v>57521.324</v>
       </c>
       <c r="G10" t="n">
-        <v>57959.25</v>
+        <v>57487.0912</v>
       </c>
       <c r="H10" t="n">
-        <v>1264.48170014687</v>
+        <v>1253.34432695792</v>
       </c>
       <c r="I10" t="n">
-        <v>1028.22535144888</v>
+        <v>1209.8527365922</v>
       </c>
       <c r="J10" t="n">
-        <v>1264.48170014687</v>
+        <v>1253.34432695792</v>
       </c>
       <c r="K10" t="s">
         <v>20</v>
@@ -8172,22 +8172,22 @@
         <v>44</v>
       </c>
       <c r="E21" t="n">
-        <v>55350.708</v>
+        <v>64105.56</v>
       </c>
       <c r="F21" t="n">
-        <v>55350.708</v>
+        <v>64331.5858</v>
       </c>
       <c r="G21" t="n">
-        <v>55350.708</v>
+        <v>64105.56</v>
       </c>
       <c r="H21" t="n">
-        <v>5917.02153301515</v>
+        <v>2214.60709266114</v>
       </c>
       <c r="I21" t="n">
-        <v>5917.02153301515</v>
+        <v>2114.88132442924</v>
       </c>
       <c r="J21" t="n">
-        <v>5917.02153301515</v>
+        <v>2214.60709266114</v>
       </c>
       <c r="K21" t="s">
         <v>20</v>
@@ -8216,22 +8216,22 @@
         <v>44</v>
       </c>
       <c r="E22" t="n">
-        <v>64817.844</v>
+        <v>55350.708</v>
       </c>
       <c r="F22" t="n">
-        <v>64854.1344</v>
+        <v>55350.708</v>
       </c>
       <c r="G22" t="n">
-        <v>64817.844</v>
+        <v>55350.708</v>
       </c>
       <c r="H22" t="n">
-        <v>2162.62587050882</v>
+        <v>5917.02153301515</v>
       </c>
       <c r="I22" t="n">
-        <v>2025.48263815248</v>
+        <v>5917.02153301515</v>
       </c>
       <c r="J22" t="n">
-        <v>2162.62587050882</v>
+        <v>5917.02153301515</v>
       </c>
       <c r="K22" t="s">
         <v>20</v>
@@ -8260,22 +8260,22 @@
         <v>44</v>
       </c>
       <c r="E23" t="n">
-        <v>64105.56</v>
+        <v>64817.844</v>
       </c>
       <c r="F23" t="n">
-        <v>64331.5858</v>
+        <v>64854.1344</v>
       </c>
       <c r="G23" t="n">
-        <v>64105.56</v>
+        <v>64817.844</v>
       </c>
       <c r="H23" t="n">
-        <v>2214.60709266114</v>
+        <v>2162.62587050882</v>
       </c>
       <c r="I23" t="n">
-        <v>2114.88132442924</v>
+        <v>2025.48263815248</v>
       </c>
       <c r="J23" t="n">
-        <v>2214.60709266114</v>
+        <v>2162.62587050882</v>
       </c>
       <c r="K23" t="s">
         <v>20</v>
@@ -8744,31 +8744,31 @@
         <v>44</v>
       </c>
       <c r="E34" t="n">
-        <v>62730.8024</v>
+        <v>49147.596</v>
       </c>
       <c r="F34" t="n">
-        <v>62730.8024</v>
+        <v>49171.35314</v>
       </c>
       <c r="G34" t="n">
-        <v>62730.8024</v>
+        <v>49147.596</v>
       </c>
       <c r="H34" t="n">
-        <v>20746.1460009376</v>
+        <v>2717.26132515061</v>
       </c>
       <c r="I34" t="n">
-        <v>20746.1460009376</v>
+        <v>2734.44430974366</v>
       </c>
       <c r="J34" t="n">
-        <v>20746.1460009376</v>
+        <v>2717.26132515061</v>
       </c>
       <c r="K34" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L34" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M34" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N34" t="s">
         <v>18</v>
@@ -8788,31 +8788,31 @@
         <v>44</v>
       </c>
       <c r="E35" t="n">
-        <v>49171.35314</v>
+        <v>62730.8024</v>
       </c>
       <c r="F35" t="n">
-        <v>49171.35314</v>
+        <v>62730.8024</v>
       </c>
       <c r="G35" t="n">
-        <v>49171.35314</v>
+        <v>62730.8024</v>
       </c>
       <c r="H35" t="n">
-        <v>2917.94605346304</v>
+        <v>20746.1460009376</v>
       </c>
       <c r="I35" t="n">
-        <v>2962.98381458141</v>
+        <v>20746.1460009376</v>
       </c>
       <c r="J35" t="n">
-        <v>2917.94605346304</v>
+        <v>20746.1460009376</v>
       </c>
       <c r="K35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N35" t="s">
         <v>18</v>
@@ -8832,22 +8832,22 @@
         <v>44</v>
       </c>
       <c r="E36" t="n">
-        <v>49147.596</v>
+        <v>49171.35314</v>
       </c>
       <c r="F36" t="n">
         <v>49171.35314</v>
       </c>
       <c r="G36" t="n">
-        <v>49147.596</v>
+        <v>49171.35314</v>
       </c>
       <c r="H36" t="n">
-        <v>2717.26132515061</v>
+        <v>2917.94605346304</v>
       </c>
       <c r="I36" t="n">
-        <v>2734.44430974366</v>
+        <v>2962.98381458141</v>
       </c>
       <c r="J36" t="n">
-        <v>2717.26132515061</v>
+        <v>2917.94605346304</v>
       </c>
       <c r="K36" t="s">
         <v>20</v>
@@ -9316,22 +9316,22 @@
         <v>44</v>
       </c>
       <c r="E47" t="n">
-        <v>53322.51</v>
+        <v>49844.955</v>
       </c>
       <c r="F47" t="n">
-        <v>53322.51</v>
+        <v>49844.955</v>
       </c>
       <c r="G47" t="n">
-        <v>53322.51</v>
+        <v>49844.955</v>
       </c>
       <c r="H47" t="n">
-        <v>9859.83185896309</v>
+        <v>1900.05386102308</v>
       </c>
       <c r="I47" t="n">
-        <v>9859.83185896309</v>
+        <v>1880.39830998911</v>
       </c>
       <c r="J47" t="n">
-        <v>9859.83185896309</v>
+        <v>1900.05386102308</v>
       </c>
       <c r="K47" t="s">
         <v>20</v>
@@ -9360,22 +9360,22 @@
         <v>44</v>
       </c>
       <c r="E48" t="n">
-        <v>50683.8836</v>
+        <v>53322.51</v>
       </c>
       <c r="F48" t="n">
-        <v>50723.904</v>
+        <v>53322.51</v>
       </c>
       <c r="G48" t="n">
-        <v>50683.8836</v>
+        <v>53322.51</v>
       </c>
       <c r="H48" t="n">
-        <v>2822.14856241887</v>
+        <v>9859.83185896309</v>
       </c>
       <c r="I48" t="n">
-        <v>2842.41542380844</v>
+        <v>9859.83185896309</v>
       </c>
       <c r="J48" t="n">
-        <v>2822.14856241887</v>
+        <v>9859.83185896309</v>
       </c>
       <c r="K48" t="s">
         <v>20</v>
@@ -9404,22 +9404,22 @@
         <v>44</v>
       </c>
       <c r="E49" t="n">
-        <v>49844.955</v>
+        <v>50683.8836</v>
       </c>
       <c r="F49" t="n">
-        <v>49844.955</v>
+        <v>50723.904</v>
       </c>
       <c r="G49" t="n">
-        <v>49844.955</v>
+        <v>50683.8836</v>
       </c>
       <c r="H49" t="n">
-        <v>1900.05386102308</v>
+        <v>2822.14856241887</v>
       </c>
       <c r="I49" t="n">
-        <v>1880.39830998911</v>
+        <v>2842.41542380844</v>
       </c>
       <c r="J49" t="n">
-        <v>1900.05386102308</v>
+        <v>2822.14856241887</v>
       </c>
       <c r="K49" t="s">
         <v>20</v>
@@ -9888,22 +9888,22 @@
         <v>44</v>
       </c>
       <c r="E60" t="n">
-        <v>48936.864</v>
+        <v>50975.9</v>
       </c>
       <c r="F60" t="n">
-        <v>48936.864</v>
+        <v>51004.14</v>
       </c>
       <c r="G60" t="n">
-        <v>48936.864</v>
+        <v>50975.9</v>
       </c>
       <c r="H60" t="n">
-        <v>8412.2346187217</v>
+        <v>2566.40103174919</v>
       </c>
       <c r="I60" t="n">
-        <v>8412.2346187217</v>
+        <v>2623.1295232966</v>
       </c>
       <c r="J60" t="n">
-        <v>8412.2346187217</v>
+        <v>2566.40103174919</v>
       </c>
       <c r="K60" t="s">
         <v>20</v>
@@ -9932,22 +9932,22 @@
         <v>44</v>
       </c>
       <c r="E61" t="n">
-        <v>50975.9</v>
+        <v>48936.864</v>
       </c>
       <c r="F61" t="n">
-        <v>50975.9</v>
+        <v>48936.864</v>
       </c>
       <c r="G61" t="n">
-        <v>50975.9</v>
+        <v>48936.864</v>
       </c>
       <c r="H61" t="n">
-        <v>3326.3870604713</v>
+        <v>8412.2346187217</v>
       </c>
       <c r="I61" t="n">
-        <v>3295.86949196496</v>
+        <v>8412.2346187217</v>
       </c>
       <c r="J61" t="n">
-        <v>3326.3870604713</v>
+        <v>8412.2346187217</v>
       </c>
       <c r="K61" t="s">
         <v>20</v>
@@ -9979,19 +9979,19 @@
         <v>50975.9</v>
       </c>
       <c r="F62" t="n">
-        <v>51004.14</v>
+        <v>50975.9</v>
       </c>
       <c r="G62" t="n">
         <v>50975.9</v>
       </c>
       <c r="H62" t="n">
-        <v>2566.40103174919</v>
+        <v>3326.3870604713</v>
       </c>
       <c r="I62" t="n">
-        <v>2623.1295232966</v>
+        <v>3295.86949196496</v>
       </c>
       <c r="J62" t="n">
-        <v>2566.40103174919</v>
+        <v>3326.3870604713</v>
       </c>
       <c r="K62" t="s">
         <v>20</v>
@@ -10518,22 +10518,22 @@
         <v>44</v>
       </c>
       <c r="E8" t="n">
-        <v>126809.76</v>
+        <v>136521.1</v>
       </c>
       <c r="F8" t="n">
-        <v>100849.095</v>
+        <v>136521.1</v>
       </c>
       <c r="G8" t="n">
-        <v>107486.368</v>
+        <v>136521.1</v>
       </c>
       <c r="H8" t="n">
-        <v>4332.25277201833</v>
+        <v>1066.12046660227</v>
       </c>
       <c r="I8" t="n">
-        <v>6428.32084072217</v>
+        <v>1085.28363716262</v>
       </c>
       <c r="J8" t="n">
-        <v>8227.9137695208</v>
+        <v>1066.12046660227</v>
       </c>
       <c r="K8" t="s">
         <v>20</v>
@@ -10562,22 +10562,22 @@
         <v>44</v>
       </c>
       <c r="E9" t="n">
-        <v>142732.52</v>
+        <v>126809.76</v>
       </c>
       <c r="F9" t="n">
-        <v>140840.9775</v>
+        <v>100849.095</v>
       </c>
       <c r="G9" t="n">
-        <v>141652.407</v>
+        <v>107486.368</v>
       </c>
       <c r="H9" t="n">
-        <v>1428.63578540444</v>
+        <v>4332.25277201833</v>
       </c>
       <c r="I9" t="n">
-        <v>1479.34869364543</v>
+        <v>6428.32084072217</v>
       </c>
       <c r="J9" t="n">
-        <v>1460.92572429665</v>
+        <v>8227.9137695208</v>
       </c>
       <c r="K9" t="s">
         <v>20</v>
@@ -10606,22 +10606,22 @@
         <v>44</v>
       </c>
       <c r="E10" t="n">
-        <v>136521.1</v>
+        <v>142732.52</v>
       </c>
       <c r="F10" t="n">
-        <v>136521.1</v>
+        <v>140840.9775</v>
       </c>
       <c r="G10" t="n">
-        <v>136521.1</v>
+        <v>141652.407</v>
       </c>
       <c r="H10" t="n">
-        <v>1066.12046660227</v>
+        <v>1428.63578540444</v>
       </c>
       <c r="I10" t="n">
-        <v>1085.28363716262</v>
+        <v>1479.34869364543</v>
       </c>
       <c r="J10" t="n">
-        <v>1066.12046660227</v>
+        <v>1460.92572429665</v>
       </c>
       <c r="K10" t="s">
         <v>20</v>
@@ -11204,22 +11204,22 @@
         <v>44</v>
       </c>
       <c r="E24" t="n">
-        <v>142834.4718</v>
+        <v>156489.975</v>
       </c>
       <c r="F24" t="n">
-        <v>109088.426</v>
+        <v>156489.975</v>
       </c>
       <c r="G24" t="n">
-        <v>122393.1359</v>
+        <v>156489.975</v>
       </c>
       <c r="H24" t="n">
-        <v>10577.2385772801</v>
+        <v>1800.43590264081</v>
       </c>
       <c r="I24" t="n">
-        <v>12096.2742091487</v>
+        <v>1788.75431262822</v>
       </c>
       <c r="J24" t="n">
-        <v>20177.7621517745</v>
+        <v>1800.43590264081</v>
       </c>
       <c r="K24" t="s">
         <v>20</v>
@@ -11248,22 +11248,22 @@
         <v>44</v>
       </c>
       <c r="E25" t="n">
-        <v>168220.47</v>
+        <v>142834.4718</v>
       </c>
       <c r="F25" t="n">
-        <v>165012.46</v>
+        <v>109088.426</v>
       </c>
       <c r="G25" t="n">
-        <v>165943.5932</v>
+        <v>122393.1359</v>
       </c>
       <c r="H25" t="n">
-        <v>2504.44178656926</v>
+        <v>10577.2385772801</v>
       </c>
       <c r="I25" t="n">
-        <v>2845.95886728038</v>
+        <v>12096.2742091487</v>
       </c>
       <c r="J25" t="n">
-        <v>2986.07009140882</v>
+        <v>20177.7621517745</v>
       </c>
       <c r="K25" t="s">
         <v>20</v>
@@ -11292,22 +11292,22 @@
         <v>44</v>
       </c>
       <c r="E26" t="n">
-        <v>156489.975</v>
+        <v>168220.47</v>
       </c>
       <c r="F26" t="n">
-        <v>156489.975</v>
+        <v>165012.46</v>
       </c>
       <c r="G26" t="n">
-        <v>156489.975</v>
+        <v>165943.5932</v>
       </c>
       <c r="H26" t="n">
-        <v>1800.43590264081</v>
+        <v>2504.44178656926</v>
       </c>
       <c r="I26" t="n">
-        <v>1788.75431262822</v>
+        <v>2845.95886728038</v>
       </c>
       <c r="J26" t="n">
-        <v>1800.43590264081</v>
+        <v>2986.07009140882</v>
       </c>
       <c r="K26" t="s">
         <v>20</v>
@@ -11890,22 +11890,22 @@
         <v>44</v>
       </c>
       <c r="E40" t="n">
-        <v>94815.174</v>
+        <v>118298.572</v>
       </c>
       <c r="F40" t="n">
-        <v>94937.2515</v>
+        <v>118298.572</v>
       </c>
       <c r="G40" t="n">
-        <v>95507.104</v>
+        <v>118298.572</v>
       </c>
       <c r="H40" t="n">
-        <v>6342.65022080927</v>
+        <v>3383.90722201948</v>
       </c>
       <c r="I40" t="n">
-        <v>14638.3239283411</v>
+        <v>3383.90722201948</v>
       </c>
       <c r="J40" t="n">
-        <v>12435.8630344971</v>
+        <v>3383.90722201948</v>
       </c>
       <c r="K40" t="s">
         <v>20</v>
@@ -11934,22 +11934,22 @@
         <v>44</v>
       </c>
       <c r="E41" t="n">
-        <v>121598.5065</v>
+        <v>94815.174</v>
       </c>
       <c r="F41" t="n">
-        <v>120771.2</v>
+        <v>94937.2515</v>
       </c>
       <c r="G41" t="n">
-        <v>121088.28</v>
+        <v>95507.104</v>
       </c>
       <c r="H41" t="n">
-        <v>3029.87727404456</v>
+        <v>6342.65022080927</v>
       </c>
       <c r="I41" t="n">
-        <v>3502.54364546422</v>
+        <v>14638.3239283411</v>
       </c>
       <c r="J41" t="n">
-        <v>3564.59376476758</v>
+        <v>12435.8630344971</v>
       </c>
       <c r="K41" t="s">
         <v>20</v>
@@ -11978,22 +11978,22 @@
         <v>44</v>
       </c>
       <c r="E42" t="n">
-        <v>118298.572</v>
+        <v>121598.5065</v>
       </c>
       <c r="F42" t="n">
-        <v>118298.572</v>
+        <v>120771.2</v>
       </c>
       <c r="G42" t="n">
-        <v>118298.572</v>
+        <v>121088.28</v>
       </c>
       <c r="H42" t="n">
-        <v>3383.90722201948</v>
+        <v>3029.87727404456</v>
       </c>
       <c r="I42" t="n">
-        <v>3383.90722201948</v>
+        <v>3502.54364546422</v>
       </c>
       <c r="J42" t="n">
-        <v>3383.90722201948</v>
+        <v>3564.59376476758</v>
       </c>
       <c r="K42" t="s">
         <v>20</v>
@@ -12576,22 +12576,22 @@
         <v>44</v>
       </c>
       <c r="E56" t="n">
-        <v>103990.836</v>
+        <v>115222.989</v>
       </c>
       <c r="F56" t="n">
-        <v>80916.704</v>
+        <v>115222.989</v>
       </c>
       <c r="G56" t="n">
-        <v>82150.088</v>
+        <v>115222.989</v>
       </c>
       <c r="H56" t="n">
-        <v>8843.18489533869</v>
+        <v>1829.92844779909</v>
       </c>
       <c r="I56" t="n">
-        <v>7753.56910572762</v>
+        <v>1841.65328029918</v>
       </c>
       <c r="J56" t="n">
-        <v>9514.16986203294</v>
+        <v>1829.92844779909</v>
       </c>
       <c r="K56" t="s">
         <v>20</v>
@@ -12620,22 +12620,22 @@
         <v>44</v>
       </c>
       <c r="E57" t="n">
-        <v>121978.912</v>
+        <v>103990.836</v>
       </c>
       <c r="F57" t="n">
-        <v>120555.24</v>
+        <v>80916.704</v>
       </c>
       <c r="G57" t="n">
-        <v>121088.28</v>
+        <v>82150.088</v>
       </c>
       <c r="H57" t="n">
-        <v>2248.58898249227</v>
+        <v>8843.18489533869</v>
       </c>
       <c r="I57" t="n">
-        <v>2103.89340159665</v>
+        <v>7753.56910572762</v>
       </c>
       <c r="J57" t="n">
-        <v>2164.21133347385</v>
+        <v>9514.16986203294</v>
       </c>
       <c r="K57" t="s">
         <v>20</v>
@@ -12664,22 +12664,22 @@
         <v>44</v>
       </c>
       <c r="E58" t="n">
-        <v>115222.989</v>
+        <v>121978.912</v>
       </c>
       <c r="F58" t="n">
-        <v>115222.989</v>
+        <v>120555.24</v>
       </c>
       <c r="G58" t="n">
-        <v>115222.989</v>
+        <v>121088.28</v>
       </c>
       <c r="H58" t="n">
-        <v>1829.92844779909</v>
+        <v>2248.58898249227</v>
       </c>
       <c r="I58" t="n">
-        <v>1841.65328029918</v>
+        <v>2103.89340159665</v>
       </c>
       <c r="J58" t="n">
-        <v>1829.92844779909</v>
+        <v>2164.21133347385</v>
       </c>
       <c r="K58" t="s">
         <v>20</v>
@@ -13262,22 +13262,22 @@
         <v>44</v>
       </c>
       <c r="E72" t="n">
-        <v>129315.219</v>
+        <v>129478.786</v>
       </c>
       <c r="F72" t="n">
-        <v>118951.428</v>
+        <v>129478.786</v>
       </c>
       <c r="G72" t="n">
-        <v>119544.998</v>
+        <v>129478.786</v>
       </c>
       <c r="H72" t="n">
-        <v>7933.14150963542</v>
+        <v>2650.9311255005</v>
       </c>
       <c r="I72" t="n">
-        <v>10525.5474188639</v>
+        <v>2650.9311255005</v>
       </c>
       <c r="J72" t="n">
-        <v>12155.1133818182</v>
+        <v>2650.9311255005</v>
       </c>
       <c r="K72" t="s">
         <v>20</v>
@@ -13306,22 +13306,22 @@
         <v>44</v>
       </c>
       <c r="E73" t="n">
-        <v>131517.822</v>
+        <v>129315.219</v>
       </c>
       <c r="F73" t="n">
-        <v>129828.72</v>
+        <v>118951.428</v>
       </c>
       <c r="G73" t="n">
-        <v>130229.258</v>
+        <v>119544.998</v>
       </c>
       <c r="H73" t="n">
-        <v>2659.93321186545</v>
+        <v>7933.14150963542</v>
       </c>
       <c r="I73" t="n">
-        <v>3072.44619562329</v>
+        <v>10525.5474188639</v>
       </c>
       <c r="J73" t="n">
-        <v>2930.76839293921</v>
+        <v>12155.1133818182</v>
       </c>
       <c r="K73" t="s">
         <v>20</v>
@@ -13350,22 +13350,22 @@
         <v>44</v>
       </c>
       <c r="E74" t="n">
-        <v>129478.786</v>
+        <v>131517.822</v>
       </c>
       <c r="F74" t="n">
-        <v>129478.786</v>
+        <v>129828.72</v>
       </c>
       <c r="G74" t="n">
-        <v>129478.786</v>
+        <v>130229.258</v>
       </c>
       <c r="H74" t="n">
-        <v>2650.9311255005</v>
+        <v>2659.93321186545</v>
       </c>
       <c r="I74" t="n">
-        <v>2650.9311255005</v>
+        <v>3072.44619562329</v>
       </c>
       <c r="J74" t="n">
-        <v>2650.9311255005</v>
+        <v>2930.76839293921</v>
       </c>
       <c r="K74" t="s">
         <v>20</v>
@@ -14006,22 +14006,22 @@
         <v>46</v>
       </c>
       <c r="E8" t="n">
-        <v>54191.89875</v>
+        <v>57959.25</v>
       </c>
       <c r="F8" t="n">
-        <v>54191.89875</v>
+        <v>57959.25</v>
       </c>
       <c r="G8" t="n">
-        <v>54191.89875</v>
+        <v>57959.25</v>
       </c>
       <c r="H8" t="n">
-        <v>3125.25308491457</v>
+        <v>1264.48170014687</v>
       </c>
       <c r="I8" t="n">
-        <v>3125.25308491457</v>
+        <v>1028.22535144888</v>
       </c>
       <c r="J8" t="n">
-        <v>3125.25308491457</v>
+        <v>1264.48170014687</v>
       </c>
       <c r="K8" t="s">
         <v>20</v>
@@ -14050,22 +14050,22 @@
         <v>46</v>
       </c>
       <c r="E9" t="n">
-        <v>57487.0912</v>
+        <v>54191.89875</v>
       </c>
       <c r="F9" t="n">
-        <v>57521.324</v>
+        <v>54191.89875</v>
       </c>
       <c r="G9" t="n">
-        <v>57487.0912</v>
+        <v>54191.89875</v>
       </c>
       <c r="H9" t="n">
-        <v>1253.34432695792</v>
+        <v>3125.25308491457</v>
       </c>
       <c r="I9" t="n">
-        <v>1209.8527365922</v>
+        <v>3125.25308491457</v>
       </c>
       <c r="J9" t="n">
-        <v>1253.34432695792</v>
+        <v>3125.25308491457</v>
       </c>
       <c r="K9" t="s">
         <v>20</v>
@@ -14094,22 +14094,22 @@
         <v>46</v>
       </c>
       <c r="E10" t="n">
-        <v>57959.25</v>
+        <v>57487.0912</v>
       </c>
       <c r="F10" t="n">
-        <v>57959.25</v>
+        <v>57521.324</v>
       </c>
       <c r="G10" t="n">
-        <v>57959.25</v>
+        <v>57487.0912</v>
       </c>
       <c r="H10" t="n">
-        <v>1264.48170014687</v>
+        <v>1253.34432695792</v>
       </c>
       <c r="I10" t="n">
-        <v>1028.22535144888</v>
+        <v>1209.8527365922</v>
       </c>
       <c r="J10" t="n">
-        <v>1264.48170014687</v>
+        <v>1253.34432695792</v>
       </c>
       <c r="K10" t="s">
         <v>20</v>
@@ -14578,22 +14578,22 @@
         <v>46</v>
       </c>
       <c r="E21" t="n">
-        <v>55350.708</v>
+        <v>64105.56</v>
       </c>
       <c r="F21" t="n">
-        <v>55350.708</v>
+        <v>64331.5858</v>
       </c>
       <c r="G21" t="n">
-        <v>55350.708</v>
+        <v>64105.56</v>
       </c>
       <c r="H21" t="n">
-        <v>5917.02153301515</v>
+        <v>2214.60709266114</v>
       </c>
       <c r="I21" t="n">
-        <v>5917.02153301515</v>
+        <v>2114.88132442924</v>
       </c>
       <c r="J21" t="n">
-        <v>5917.02153301515</v>
+        <v>2214.60709266114</v>
       </c>
       <c r="K21" t="s">
         <v>20</v>
@@ -14622,22 +14622,22 @@
         <v>46</v>
       </c>
       <c r="E22" t="n">
-        <v>64817.844</v>
+        <v>55350.708</v>
       </c>
       <c r="F22" t="n">
-        <v>64854.1344</v>
+        <v>55350.708</v>
       </c>
       <c r="G22" t="n">
-        <v>64817.844</v>
+        <v>55350.708</v>
       </c>
       <c r="H22" t="n">
-        <v>2162.62587050882</v>
+        <v>5917.02153301515</v>
       </c>
       <c r="I22" t="n">
-        <v>2025.48263815248</v>
+        <v>5917.02153301515</v>
       </c>
       <c r="J22" t="n">
-        <v>2162.62587050882</v>
+        <v>5917.02153301515</v>
       </c>
       <c r="K22" t="s">
         <v>20</v>
@@ -14666,22 +14666,22 @@
         <v>46</v>
       </c>
       <c r="E23" t="n">
-        <v>64105.56</v>
+        <v>64817.844</v>
       </c>
       <c r="F23" t="n">
-        <v>64331.5858</v>
+        <v>64854.1344</v>
       </c>
       <c r="G23" t="n">
-        <v>64105.56</v>
+        <v>64817.844</v>
       </c>
       <c r="H23" t="n">
-        <v>2214.60709266114</v>
+        <v>2162.62587050882</v>
       </c>
       <c r="I23" t="n">
-        <v>2114.88132442924</v>
+        <v>2025.48263815248</v>
       </c>
       <c r="J23" t="n">
-        <v>2214.60709266114</v>
+        <v>2162.62587050882</v>
       </c>
       <c r="K23" t="s">
         <v>20</v>
@@ -15150,31 +15150,31 @@
         <v>46</v>
       </c>
       <c r="E34" t="n">
-        <v>62730.8024</v>
+        <v>49147.596</v>
       </c>
       <c r="F34" t="n">
-        <v>62730.8024</v>
+        <v>49171.35314</v>
       </c>
       <c r="G34" t="n">
-        <v>62730.8024</v>
+        <v>49147.596</v>
       </c>
       <c r="H34" t="n">
-        <v>20746.1460009376</v>
+        <v>2717.26132515061</v>
       </c>
       <c r="I34" t="n">
-        <v>20746.1460009376</v>
+        <v>2734.44430974366</v>
       </c>
       <c r="J34" t="n">
-        <v>20746.1460009376</v>
+        <v>2717.26132515061</v>
       </c>
       <c r="K34" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L34" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M34" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N34" t="s">
         <v>18</v>
@@ -15194,31 +15194,31 @@
         <v>46</v>
       </c>
       <c r="E35" t="n">
-        <v>49171.35314</v>
+        <v>62730.8024</v>
       </c>
       <c r="F35" t="n">
-        <v>49171.35314</v>
+        <v>62730.8024</v>
       </c>
       <c r="G35" t="n">
-        <v>49171.35314</v>
+        <v>62730.8024</v>
       </c>
       <c r="H35" t="n">
-        <v>2917.94605346304</v>
+        <v>20746.1460009376</v>
       </c>
       <c r="I35" t="n">
-        <v>2962.98381458141</v>
+        <v>20746.1460009376</v>
       </c>
       <c r="J35" t="n">
-        <v>2917.94605346304</v>
+        <v>20746.1460009376</v>
       </c>
       <c r="K35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N35" t="s">
         <v>18</v>
@@ -15238,22 +15238,22 @@
         <v>46</v>
       </c>
       <c r="E36" t="n">
-        <v>49147.596</v>
+        <v>49171.35314</v>
       </c>
       <c r="F36" t="n">
         <v>49171.35314</v>
       </c>
       <c r="G36" t="n">
-        <v>49147.596</v>
+        <v>49171.35314</v>
       </c>
       <c r="H36" t="n">
-        <v>2717.26132515061</v>
+        <v>2917.94605346304</v>
       </c>
       <c r="I36" t="n">
-        <v>2734.44430974366</v>
+        <v>2962.98381458141</v>
       </c>
       <c r="J36" t="n">
-        <v>2717.26132515061</v>
+        <v>2917.94605346304</v>
       </c>
       <c r="K36" t="s">
         <v>20</v>
@@ -15722,22 +15722,22 @@
         <v>46</v>
       </c>
       <c r="E47" t="n">
-        <v>53322.51</v>
+        <v>49844.955</v>
       </c>
       <c r="F47" t="n">
-        <v>53322.51</v>
+        <v>49844.955</v>
       </c>
       <c r="G47" t="n">
-        <v>53322.51</v>
+        <v>49844.955</v>
       </c>
       <c r="H47" t="n">
-        <v>9859.83185896309</v>
+        <v>1900.05386102308</v>
       </c>
       <c r="I47" t="n">
-        <v>9859.83185896309</v>
+        <v>1880.39830998911</v>
       </c>
       <c r="J47" t="n">
-        <v>9859.83185896309</v>
+        <v>1900.05386102308</v>
       </c>
       <c r="K47" t="s">
         <v>20</v>
@@ -15766,22 +15766,22 @@
         <v>46</v>
       </c>
       <c r="E48" t="n">
-        <v>50683.8836</v>
+        <v>53322.51</v>
       </c>
       <c r="F48" t="n">
-        <v>50723.904</v>
+        <v>53322.51</v>
       </c>
       <c r="G48" t="n">
-        <v>50683.8836</v>
+        <v>53322.51</v>
       </c>
       <c r="H48" t="n">
-        <v>2822.14856241887</v>
+        <v>9859.83185896309</v>
       </c>
       <c r="I48" t="n">
-        <v>2842.41542380844</v>
+        <v>9859.83185896309</v>
       </c>
       <c r="J48" t="n">
-        <v>2822.14856241887</v>
+        <v>9859.83185896309</v>
       </c>
       <c r="K48" t="s">
         <v>20</v>
@@ -15810,22 +15810,22 @@
         <v>46</v>
       </c>
       <c r="E49" t="n">
-        <v>49844.955</v>
+        <v>50683.8836</v>
       </c>
       <c r="F49" t="n">
-        <v>49844.955</v>
+        <v>50723.904</v>
       </c>
       <c r="G49" t="n">
-        <v>49844.955</v>
+        <v>50683.8836</v>
       </c>
       <c r="H49" t="n">
-        <v>1900.05386102308</v>
+        <v>2822.14856241887</v>
       </c>
       <c r="I49" t="n">
-        <v>1880.39830998911</v>
+        <v>2842.41542380844</v>
       </c>
       <c r="J49" t="n">
-        <v>1900.05386102308</v>
+        <v>2822.14856241887</v>
       </c>
       <c r="K49" t="s">
         <v>20</v>
@@ -16294,22 +16294,22 @@
         <v>46</v>
       </c>
       <c r="E60" t="n">
-        <v>48936.864</v>
+        <v>50975.9</v>
       </c>
       <c r="F60" t="n">
-        <v>48936.864</v>
+        <v>51004.14</v>
       </c>
       <c r="G60" t="n">
-        <v>48936.864</v>
+        <v>50975.9</v>
       </c>
       <c r="H60" t="n">
-        <v>8412.2346187217</v>
+        <v>2566.40103174919</v>
       </c>
       <c r="I60" t="n">
-        <v>8412.2346187217</v>
+        <v>2623.1295232966</v>
       </c>
       <c r="J60" t="n">
-        <v>8412.2346187217</v>
+        <v>2566.40103174919</v>
       </c>
       <c r="K60" t="s">
         <v>20</v>
@@ -16338,22 +16338,22 @@
         <v>46</v>
       </c>
       <c r="E61" t="n">
-        <v>50975.9</v>
+        <v>48936.864</v>
       </c>
       <c r="F61" t="n">
-        <v>50975.9</v>
+        <v>48936.864</v>
       </c>
       <c r="G61" t="n">
-        <v>50975.9</v>
+        <v>48936.864</v>
       </c>
       <c r="H61" t="n">
-        <v>3326.3870604713</v>
+        <v>8412.2346187217</v>
       </c>
       <c r="I61" t="n">
-        <v>3295.86949196496</v>
+        <v>8412.2346187217</v>
       </c>
       <c r="J61" t="n">
-        <v>3326.3870604713</v>
+        <v>8412.2346187217</v>
       </c>
       <c r="K61" t="s">
         <v>20</v>
@@ -16385,19 +16385,19 @@
         <v>50975.9</v>
       </c>
       <c r="F62" t="n">
-        <v>51004.14</v>
+        <v>50975.9</v>
       </c>
       <c r="G62" t="n">
         <v>50975.9</v>
       </c>
       <c r="H62" t="n">
-        <v>2566.40103174919</v>
+        <v>3326.3870604713</v>
       </c>
       <c r="I62" t="n">
-        <v>2623.1295232966</v>
+        <v>3295.86949196496</v>
       </c>
       <c r="J62" t="n">
-        <v>2566.40103174919</v>
+        <v>3326.3870604713</v>
       </c>
       <c r="K62" t="s">
         <v>20</v>
@@ -16924,22 +16924,22 @@
         <v>46</v>
       </c>
       <c r="E8" t="n">
-        <v>126809.76</v>
+        <v>136521.1</v>
       </c>
       <c r="F8" t="n">
-        <v>100849.095</v>
+        <v>136521.1</v>
       </c>
       <c r="G8" t="n">
-        <v>107486.368</v>
+        <v>136521.1</v>
       </c>
       <c r="H8" t="n">
-        <v>4332.25277201833</v>
+        <v>1066.12046660227</v>
       </c>
       <c r="I8" t="n">
-        <v>6428.32084072217</v>
+        <v>1085.28363716262</v>
       </c>
       <c r="J8" t="n">
-        <v>8227.9137695208</v>
+        <v>1066.12046660227</v>
       </c>
       <c r="K8" t="s">
         <v>20</v>
@@ -16968,22 +16968,22 @@
         <v>46</v>
       </c>
       <c r="E9" t="n">
-        <v>142732.52</v>
+        <v>126809.76</v>
       </c>
       <c r="F9" t="n">
-        <v>140840.9775</v>
+        <v>100849.095</v>
       </c>
       <c r="G9" t="n">
-        <v>141652.407</v>
+        <v>107486.368</v>
       </c>
       <c r="H9" t="n">
-        <v>1428.63578540444</v>
+        <v>4332.25277201833</v>
       </c>
       <c r="I9" t="n">
-        <v>1479.34869364543</v>
+        <v>6428.32084072217</v>
       </c>
       <c r="J9" t="n">
-        <v>1460.92572429665</v>
+        <v>8227.9137695208</v>
       </c>
       <c r="K9" t="s">
         <v>20</v>
@@ -17012,22 +17012,22 @@
         <v>46</v>
       </c>
       <c r="E10" t="n">
-        <v>136521.1</v>
+        <v>142732.52</v>
       </c>
       <c r="F10" t="n">
-        <v>136521.1</v>
+        <v>140840.9775</v>
       </c>
       <c r="G10" t="n">
-        <v>136521.1</v>
+        <v>141652.407</v>
       </c>
       <c r="H10" t="n">
-        <v>1066.12046660227</v>
+        <v>1428.63578540444</v>
       </c>
       <c r="I10" t="n">
-        <v>1085.28363716262</v>
+        <v>1479.34869364543</v>
       </c>
       <c r="J10" t="n">
-        <v>1066.12046660227</v>
+        <v>1460.92572429665</v>
       </c>
       <c r="K10" t="s">
         <v>20</v>
@@ -17572,22 +17572,22 @@
         <v>46</v>
       </c>
       <c r="E23" t="n">
-        <v>142834.4718</v>
+        <v>156489.975</v>
       </c>
       <c r="F23" t="n">
-        <v>109088.426</v>
+        <v>156489.975</v>
       </c>
       <c r="G23" t="n">
-        <v>122393.1359</v>
+        <v>156489.975</v>
       </c>
       <c r="H23" t="n">
-        <v>10577.2385772801</v>
+        <v>1800.43590264081</v>
       </c>
       <c r="I23" t="n">
-        <v>12096.2742091487</v>
+        <v>1788.75431262822</v>
       </c>
       <c r="J23" t="n">
-        <v>20177.7621517745</v>
+        <v>1800.43590264081</v>
       </c>
       <c r="K23" t="s">
         <v>20</v>
@@ -17616,22 +17616,22 @@
         <v>46</v>
       </c>
       <c r="E24" t="n">
-        <v>168220.47</v>
+        <v>142834.4718</v>
       </c>
       <c r="F24" t="n">
-        <v>165012.46</v>
+        <v>109088.426</v>
       </c>
       <c r="G24" t="n">
-        <v>165943.5932</v>
+        <v>122393.1359</v>
       </c>
       <c r="H24" t="n">
-        <v>2504.44178656926</v>
+        <v>10577.2385772801</v>
       </c>
       <c r="I24" t="n">
-        <v>2845.95886728038</v>
+        <v>12096.2742091487</v>
       </c>
       <c r="J24" t="n">
-        <v>2986.07009140882</v>
+        <v>20177.7621517745</v>
       </c>
       <c r="K24" t="s">
         <v>20</v>
@@ -17660,22 +17660,22 @@
         <v>46</v>
       </c>
       <c r="E25" t="n">
-        <v>156489.975</v>
+        <v>168220.47</v>
       </c>
       <c r="F25" t="n">
-        <v>156489.975</v>
+        <v>165012.46</v>
       </c>
       <c r="G25" t="n">
-        <v>156489.975</v>
+        <v>165943.5932</v>
       </c>
       <c r="H25" t="n">
-        <v>1800.43590264081</v>
+        <v>2504.44178656926</v>
       </c>
       <c r="I25" t="n">
-        <v>1788.75431262822</v>
+        <v>2845.95886728038</v>
       </c>
       <c r="J25" t="n">
-        <v>1800.43590264081</v>
+        <v>2986.07009140882</v>
       </c>
       <c r="K25" t="s">
         <v>20</v>
@@ -18220,22 +18220,22 @@
         <v>46</v>
       </c>
       <c r="E38" t="n">
-        <v>94815.174</v>
+        <v>118298.572</v>
       </c>
       <c r="F38" t="n">
-        <v>94937.2515</v>
+        <v>118298.572</v>
       </c>
       <c r="G38" t="n">
-        <v>95507.104</v>
+        <v>118298.572</v>
       </c>
       <c r="H38" t="n">
-        <v>6342.65022080927</v>
+        <v>3383.90722201948</v>
       </c>
       <c r="I38" t="n">
-        <v>14638.3239283411</v>
+        <v>3383.90722201948</v>
       </c>
       <c r="J38" t="n">
-        <v>12435.8630344971</v>
+        <v>3383.90722201948</v>
       </c>
       <c r="K38" t="s">
         <v>20</v>
@@ -18264,22 +18264,22 @@
         <v>46</v>
       </c>
       <c r="E39" t="n">
-        <v>121598.5065</v>
+        <v>94815.174</v>
       </c>
       <c r="F39" t="n">
-        <v>120771.2</v>
+        <v>94937.2515</v>
       </c>
       <c r="G39" t="n">
-        <v>121088.28</v>
+        <v>95507.104</v>
       </c>
       <c r="H39" t="n">
-        <v>3029.87727404456</v>
+        <v>6342.65022080927</v>
       </c>
       <c r="I39" t="n">
-        <v>3502.54364546422</v>
+        <v>14638.3239283411</v>
       </c>
       <c r="J39" t="n">
-        <v>3564.59376476758</v>
+        <v>12435.8630344971</v>
       </c>
       <c r="K39" t="s">
         <v>20</v>
@@ -18308,22 +18308,22 @@
         <v>46</v>
       </c>
       <c r="E40" t="n">
-        <v>118298.572</v>
+        <v>121598.5065</v>
       </c>
       <c r="F40" t="n">
-        <v>118298.572</v>
+        <v>120771.2</v>
       </c>
       <c r="G40" t="n">
-        <v>118298.572</v>
+        <v>121088.28</v>
       </c>
       <c r="H40" t="n">
-        <v>3383.90722201948</v>
+        <v>3029.87727404456</v>
       </c>
       <c r="I40" t="n">
-        <v>3383.90722201948</v>
+        <v>3502.54364546422</v>
       </c>
       <c r="J40" t="n">
-        <v>3383.90722201948</v>
+        <v>3564.59376476758</v>
       </c>
       <c r="K40" t="s">
         <v>20</v>
@@ -18868,22 +18868,22 @@
         <v>46</v>
       </c>
       <c r="E53" t="n">
-        <v>103990.836</v>
+        <v>115222.989</v>
       </c>
       <c r="F53" t="n">
-        <v>80916.704</v>
+        <v>115222.989</v>
       </c>
       <c r="G53" t="n">
-        <v>82150.088</v>
+        <v>115222.989</v>
       </c>
       <c r="H53" t="n">
-        <v>8843.18489533869</v>
+        <v>1829.92844779909</v>
       </c>
       <c r="I53" t="n">
-        <v>7753.56910572762</v>
+        <v>1841.65328029918</v>
       </c>
       <c r="J53" t="n">
-        <v>9514.16986203294</v>
+        <v>1829.92844779909</v>
       </c>
       <c r="K53" t="s">
         <v>20</v>
@@ -18912,22 +18912,22 @@
         <v>46</v>
       </c>
       <c r="E54" t="n">
-        <v>121978.912</v>
+        <v>103990.836</v>
       </c>
       <c r="F54" t="n">
-        <v>120555.24</v>
+        <v>80916.704</v>
       </c>
       <c r="G54" t="n">
-        <v>121088.28</v>
+        <v>82150.088</v>
       </c>
       <c r="H54" t="n">
-        <v>2248.58898249227</v>
+        <v>8843.18489533869</v>
       </c>
       <c r="I54" t="n">
-        <v>2103.89340159665</v>
+        <v>7753.56910572762</v>
       </c>
       <c r="J54" t="n">
-        <v>2164.21133347385</v>
+        <v>9514.16986203294</v>
       </c>
       <c r="K54" t="s">
         <v>20</v>
@@ -18956,22 +18956,22 @@
         <v>46</v>
       </c>
       <c r="E55" t="n">
-        <v>115222.989</v>
+        <v>121978.912</v>
       </c>
       <c r="F55" t="n">
-        <v>115222.989</v>
+        <v>120555.24</v>
       </c>
       <c r="G55" t="n">
-        <v>115222.989</v>
+        <v>121088.28</v>
       </c>
       <c r="H55" t="n">
-        <v>1829.92844779909</v>
+        <v>2248.58898249227</v>
       </c>
       <c r="I55" t="n">
-        <v>1841.65328029918</v>
+        <v>2103.89340159665</v>
       </c>
       <c r="J55" t="n">
-        <v>1829.92844779909</v>
+        <v>2164.21133347385</v>
       </c>
       <c r="K55" t="s">
         <v>20</v>
@@ -19516,22 +19516,22 @@
         <v>46</v>
       </c>
       <c r="E68" t="n">
-        <v>129315.219</v>
+        <v>129478.786</v>
       </c>
       <c r="F68" t="n">
-        <v>118951.428</v>
+        <v>129478.786</v>
       </c>
       <c r="G68" t="n">
-        <v>119544.998</v>
+        <v>129478.786</v>
       </c>
       <c r="H68" t="n">
-        <v>7933.14150963542</v>
+        <v>2650.9311255005</v>
       </c>
       <c r="I68" t="n">
-        <v>10525.5474188639</v>
+        <v>2650.9311255005</v>
       </c>
       <c r="J68" t="n">
-        <v>12155.1133818182</v>
+        <v>2650.9311255005</v>
       </c>
       <c r="K68" t="s">
         <v>20</v>
@@ -19560,22 +19560,22 @@
         <v>46</v>
       </c>
       <c r="E69" t="n">
-        <v>131517.822</v>
+        <v>129315.219</v>
       </c>
       <c r="F69" t="n">
-        <v>129828.72</v>
+        <v>118951.428</v>
       </c>
       <c r="G69" t="n">
-        <v>130229.258</v>
+        <v>119544.998</v>
       </c>
       <c r="H69" t="n">
-        <v>2659.93321186545</v>
+        <v>7933.14150963542</v>
       </c>
       <c r="I69" t="n">
-        <v>3072.44619562329</v>
+        <v>10525.5474188639</v>
       </c>
       <c r="J69" t="n">
-        <v>2930.76839293921</v>
+        <v>12155.1133818182</v>
       </c>
       <c r="K69" t="s">
         <v>20</v>
@@ -19604,22 +19604,22 @@
         <v>46</v>
       </c>
       <c r="E70" t="n">
-        <v>129478.786</v>
+        <v>131517.822</v>
       </c>
       <c r="F70" t="n">
-        <v>129478.786</v>
+        <v>129828.72</v>
       </c>
       <c r="G70" t="n">
-        <v>129478.786</v>
+        <v>130229.258</v>
       </c>
       <c r="H70" t="n">
-        <v>2650.9311255005</v>
+        <v>2659.93321186545</v>
       </c>
       <c r="I70" t="n">
-        <v>2650.9311255005</v>
+        <v>3072.44619562329</v>
       </c>
       <c r="J70" t="n">
-        <v>2650.9311255005</v>
+        <v>2930.76839293921</v>
       </c>
       <c r="K70" t="s">
         <v>20</v>

</xml_diff>